<commit_message>
getting good at tree traversal
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\LeetCodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB737B8-8F6E-4861-8E11-F471D12EA613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBA2819-FF0F-4475-853D-51BB579C5C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
+    <workbookView xWindow="2250" yWindow="1905" windowWidth="14460" windowHeight="12720" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>day</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/symmetric-tree/submissions/1062657334/</t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-depth-of-binary-tree/submissions/1063310024/</t>
   </si>
 </sst>
 </file>
@@ -591,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECC8050-3973-4D61-AD7A-348E46DD3771}">
   <dimension ref="A2:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,6 +1188,30 @@
       <c r="A23">
         <v>21</v>
       </c>
+      <c r="B23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>45</v>
+      </c>
+      <c r="F23">
+        <v>0.35</v>
+      </c>
+      <c r="G23">
+        <v>18.7</v>
+      </c>
+      <c r="H23">
+        <v>0.47</v>
+      </c>
+      <c r="I23" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1246,6 +1276,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B22" r:id="rId1" display="https://leetcode.com/problems/symmetric-tree/" xr:uid="{179A0BEC-6488-4641-A2CB-0D9767BAF139}"/>
+    <hyperlink ref="B23" r:id="rId2" display="https://leetcode.com/problems/maximum-depth-of-binary-tree" xr:uid="{6902DA6B-21B5-44D4-A518-15AE37E860B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1295,27 +1326,27 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(Sheet1!C3:C500)/COUNT(Sheet1!C3:C500)</f>
-        <v>0.85</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(Sheet1!D3:D500)/COUNT(Sheet1!D3:D500)</f>
-        <v>1.8235294117647058</v>
+        <v>1.8888888888888888</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(Sheet1!E3:E500)/COUNT(Sheet1!E3:E500)</f>
-        <v>190.8235294117647</v>
+        <v>182.72222222222223</v>
       </c>
       <c r="E3" s="2">
         <f>SUM(Sheet1!F3:F500)/COUNT(Sheet1!F3:F500)</f>
-        <v>0.47941176470588237</v>
+        <v>0.47222222222222221</v>
       </c>
       <c r="F3" s="2">
         <f>SUM(Sheet1!G3:G500)/COUNT(Sheet1!G3:G500)</f>
-        <v>16.351764705882349</v>
+        <v>16.482222222222219</v>
       </c>
       <c r="G3" s="2">
         <f>SUM(Sheet1!H3:H500)/COUNT(Sheet1!H3:H500)</f>
-        <v>0.28397058823529409</v>
+        <v>0.29430555555555554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
need more practice in BTS
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\LeetCodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF9A210-EC6A-478D-B4D0-700EA69EE079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02A43CA-680F-4BE9-B9E7-FD6C99239DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
+    <workbookView xWindow="9885" yWindow="1515" windowWidth="14460" windowHeight="12720" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>day</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Convert Sorted Array to Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Balanced Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -600,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECC8050-3973-4D61-AD7A-348E46DD3771}">
   <dimension ref="A2:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,6 +1234,12 @@
       <c r="A25">
         <v>23</v>
       </c>
+      <c r="B25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1287,6 +1296,7 @@
     <hyperlink ref="B22" r:id="rId1" display="https://leetcode.com/problems/symmetric-tree/" xr:uid="{179A0BEC-6488-4641-A2CB-0D9767BAF139}"/>
     <hyperlink ref="B23" r:id="rId2" display="https://leetcode.com/problems/maximum-depth-of-binary-tree" xr:uid="{6902DA6B-21B5-44D4-A518-15AE37E860B6}"/>
     <hyperlink ref="B24" r:id="rId3" display="https://leetcode.com/problems/convert-sorted-array-to-binary-search-tree/" xr:uid="{2BB159B6-E93E-4022-A9CD-2B613846B527}"/>
+    <hyperlink ref="B25" r:id="rId4" display="https://leetcode.com/problems/balanced-binary-tree/" xr:uid="{83488FFA-404E-4890-9EA2-D1ECF37FB47D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1336,7 +1346,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(Sheet1!C3:C500)/COUNT(Sheet1!C3:C500)</f>
-        <v>0.81818181818181823</v>
+        <v>0.78260869565217395</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(Sheet1!D3:D500)/COUNT(Sheet1!D3:D500)</f>

</xml_diff>

<commit_message>
getting familiar with tree traversal
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\LeetCodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C4E9CC-CF94-4A62-939C-D11E335BB615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C178D4-B7F1-46B0-910C-9F62CD6C1AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
+    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15720" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>day</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/binary-tree-preorder-traversal/submissions/</t>
+  </si>
+  <si>
+    <t>Binary Tree Postorder Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-postorder-traversal/submissions/</t>
   </si>
 </sst>
 </file>
@@ -646,7 +652,7 @@
   <dimension ref="A2:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,6 +1489,30 @@
       <c r="A34">
         <v>32</v>
       </c>
+      <c r="B34" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>34</v>
+      </c>
+      <c r="F34">
+        <v>0.19</v>
+      </c>
+      <c r="G34">
+        <v>16.09</v>
+      </c>
+      <c r="H34">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="I34" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -1503,6 +1533,7 @@
     <hyperlink ref="B31" r:id="rId10" display="https://leetcode.com/problems/single-number/" xr:uid="{A88A07CF-84E9-4F40-8560-789C74C67FBA}"/>
     <hyperlink ref="B32" r:id="rId11" display="https://leetcode.com/problems/linked-list-cycle/" xr:uid="{E1A8F251-1548-46DD-B80B-75DF44348844}"/>
     <hyperlink ref="B33" r:id="rId12" display="https://leetcode.com/problems/binary-tree-preorder-traversal/" xr:uid="{385B877C-E859-424E-841A-ABD6E6139F49}"/>
+    <hyperlink ref="B34" r:id="rId13" display="https://leetcode.com/problems/binary-tree-postorder-traversal/" xr:uid="{791124EC-361F-4D29-BFC1-EB95676DE037}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1552,27 +1583,27 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(Sheet1!C3:C500)/COUNT(Sheet1!C3:C500)</f>
-        <v>0.77419354838709675</v>
+        <v>0.78125</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(Sheet1!D3:D500)/COUNT(Sheet1!D3:D500)</f>
-        <v>1.6666666666666667</v>
+        <v>1.64</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(Sheet1!E3:E500)/COUNT(Sheet1!E3:E500)</f>
-        <v>167.08333333333334</v>
+        <v>161.76</v>
       </c>
       <c r="E3" s="2">
         <f>SUM(Sheet1!F3:F500)/COUNT(Sheet1!F3:F500)</f>
-        <v>0.44560833333333333</v>
+        <v>0.43538399999999994</v>
       </c>
       <c r="F3" s="2">
         <f>SUM(Sheet1!G3:G500)/COUNT(Sheet1!G3:G500)</f>
-        <v>18.310833333333331</v>
+        <v>18.221999999999998</v>
       </c>
       <c r="G3" s="2">
         <f>SUM(Sheet1!H3:H500)/COUNT(Sheet1!H3:H500)</f>
-        <v>0.32469999999999993</v>
+        <v>0.31257999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sql inner vs left
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\LeetCodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E85C72B-F1DB-4307-93C0-B648648EFD34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE0F65D-694A-4EFF-A62A-3CB7F3096D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
+    <workbookView xWindow="2430" yWindow="2490" windowWidth="21600" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>day</t>
   </si>
@@ -295,6 +295,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/combine-two-tables/submissions/</t>
+  </si>
+  <si>
+    <t>Employees Earning More Than Their Managers</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/employees-earning-more-than-their-managers/submissions/</t>
   </si>
 </sst>
 </file>
@@ -676,15 +682,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECC8050-3973-4D61-AD7A-348E46DD3771}">
-  <dimension ref="A2:J39"/>
+  <dimension ref="A2:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
@@ -1648,6 +1654,26 @@
       </c>
       <c r="I39" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>612</v>
+      </c>
+      <c r="F40">
+        <v>4.8099999999999997E-2</v>
+      </c>
+      <c r="I40" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1670,6 +1696,7 @@
     <hyperlink ref="B37" r:id="rId16" display="https://leetcode.com/problems/majority-element/" xr:uid="{98274804-AC11-4B76-A3B6-81F0C81B91DE}"/>
     <hyperlink ref="B38" r:id="rId17" display="https://leetcode.com/problems/excel-sheet-column-number/" xr:uid="{7F28BEC0-D155-4F70-8ACF-323F45BBCBBB}"/>
     <hyperlink ref="B39" r:id="rId18" display="https://leetcode.com/problems/combine-two-tables/" xr:uid="{984C0F2F-EFB7-4993-AA93-319437E6DC97}"/>
+    <hyperlink ref="B40" r:id="rId19" display="https://leetcode.com/problems/employees-earning-more-than-their-managers/" xr:uid="{62307ADD-7C06-419F-B09F-30D3997943C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1719,19 +1746,19 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(Sheet1!C3:C500)/COUNT(Sheet1!C3:C500)</f>
-        <v>0.78378378378378377</v>
+        <v>0.78947368421052633</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(Sheet1!D3:D500)/COUNT(Sheet1!D3:D500)</f>
-        <v>1.5517241379310345</v>
+        <v>1.5333333333333334</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(Sheet1!E3:E500)/COUNT(Sheet1!E3:E500)</f>
-        <v>173.10344827586206</v>
+        <v>187.73333333333332</v>
       </c>
       <c r="E3" s="2">
         <f>SUM(Sheet1!F3:F500)/COUNT(Sheet1!F3:F500)</f>
-        <v>0.41422413793103446</v>
+        <v>0.40201999999999999</v>
       </c>
       <c r="F3" s="2">
         <f>SUM(Sheet1!G3:G500)/COUNT(Sheet1!G3:G500)</f>

</xml_diff>

<commit_message>
learned another use of zip and set
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DAAF71-0487-449A-A844-6B7E3416133E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2CA5F1-C509-4B97-AF16-0FAD85E43D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="2205" windowWidth="21600" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>day</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/remove-linked-list-elements/submissions/1086397533/</t>
+  </si>
+  <si>
+    <t>Isomorphic Strings</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/isomorphic-strings/submissions/1087078218/</t>
   </si>
 </sst>
 </file>
@@ -739,7 +745,7 @@
   <dimension ref="A2:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1978,6 +1984,30 @@
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>46</v>
+      </c>
+      <c r="F51">
+        <v>0.4</v>
+      </c>
+      <c r="G51">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="H51">
+        <v>0.42</v>
+      </c>
+      <c r="I51" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2051,9 +2081,10 @@
     <hyperlink ref="B48" r:id="rId27" display="https://leetcode.com/problems/rising-temperature/" xr:uid="{59B31695-C530-45E4-A1E0-820944B1212E}"/>
     <hyperlink ref="B49" r:id="rId28" display="https://leetcode.com/problems/happy-number/" xr:uid="{AE195737-CD70-47F3-906B-F94ED634ED2D}"/>
     <hyperlink ref="B50" r:id="rId29" display="https://leetcode.com/problems/remove-linked-list-elements/" xr:uid="{5845B5FD-7CAF-4F79-8741-3AAD834B48D0}"/>
+    <hyperlink ref="B51" r:id="rId30" display="https://leetcode.com/problems/isomorphic-strings/" xr:uid="{05553CA3-8DF4-4719-8B18-370E9DB50A1C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
 
@@ -2101,27 +2132,27 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.78723404255319152</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>
-        <v>1.5675675675675675</v>
+        <v>1.5526315789473684</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(List!E3:E500)/COUNT(List!E3:E500)</f>
-        <v>231.08108108108109</v>
+        <v>226.21052631578948</v>
       </c>
       <c r="E3" s="2">
         <f>SUM(List!F3:F500)/COUNT(List!F3:F500)</f>
-        <v>0.42325945945945936</v>
+        <v>0.42264736842105255</v>
       </c>
       <c r="F3" s="2">
         <f>SUM(List!G3:G500)/COUNT(List!G3:G500)</f>
-        <v>22.366176470588236</v>
+        <v>22.201428571428572</v>
       </c>
       <c r="G3" s="2">
         <f>SUM(List!H3:H500)/COUNT(List!H3:H500)</f>
-        <v>0.35144117647058826</v>
+        <v>0.35339999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
readme and file path managed
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2CA5F1-C509-4B97-AF16-0FAD85E43D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258DBC19-9AA6-41C8-B7F4-C17FB26C836B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
+    <workbookView xWindow="7755" yWindow="2415" windowWidth="21600" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -745,7 +745,7 @@
   <dimension ref="A2:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,7 +2093,7 @@
   <dimension ref="A2:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
aimed completion in 5 min
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258DBC19-9AA6-41C8-B7F4-C17FB26C836B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2927CA9-D304-42CD-B661-C4C07E9D2FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7755" yWindow="2415" windowWidth="21600" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
+    <workbookView xWindow="4245" yWindow="2325" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>day</t>
   </si>
@@ -361,6 +361,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/isomorphic-strings/submissions/1087078218/</t>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-linked-list/submissions/1088037333/</t>
   </si>
 </sst>
 </file>
@@ -744,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECC8050-3973-4D61-AD7A-348E46DD3771}">
   <dimension ref="A2:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,6 +2019,30 @@
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>54</v>
+      </c>
+      <c r="F52">
+        <v>0.92</v>
+      </c>
+      <c r="G52">
+        <v>18.7</v>
+      </c>
+      <c r="H52">
+        <v>0.83</v>
+      </c>
+      <c r="I52" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2082,9 +2112,10 @@
     <hyperlink ref="B49" r:id="rId28" display="https://leetcode.com/problems/happy-number/" xr:uid="{AE195737-CD70-47F3-906B-F94ED634ED2D}"/>
     <hyperlink ref="B50" r:id="rId29" display="https://leetcode.com/problems/remove-linked-list-elements/" xr:uid="{5845B5FD-7CAF-4F79-8741-3AAD834B48D0}"/>
     <hyperlink ref="B51" r:id="rId30" display="https://leetcode.com/problems/isomorphic-strings/" xr:uid="{05553CA3-8DF4-4719-8B18-370E9DB50A1C}"/>
+    <hyperlink ref="B52" r:id="rId31" display="https://leetcode.com/problems/reverse-linked-list/" xr:uid="{64BAC716-BDC1-4071-B01E-7D14E2F1B268}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 
@@ -2092,7 +2123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474C32BF-24AC-4A70-BA6A-73A9C2809AF6}">
   <dimension ref="A2:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -2132,27 +2163,27 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.79166666666666663</v>
+        <v>0.79591836734693877</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>
-        <v>1.5526315789473684</v>
+        <v>1.5384615384615385</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(List!E3:E500)/COUNT(List!E3:E500)</f>
-        <v>226.21052631578948</v>
+        <v>221.7948717948718</v>
       </c>
       <c r="E3" s="2">
         <f>SUM(List!F3:F500)/COUNT(List!F3:F500)</f>
-        <v>0.42264736842105255</v>
+        <v>0.43539999999999995</v>
       </c>
       <c r="F3" s="2">
         <f>SUM(List!G3:G500)/COUNT(List!G3:G500)</f>
-        <v>22.201428571428572</v>
+        <v>22.104166666666671</v>
       </c>
       <c r="G3" s="2">
         <f>SUM(List!H3:H500)/COUNT(List!H3:H500)</f>
-        <v>0.35339999999999999</v>
+        <v>0.3666388888888889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
need more study in tree algo
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EF8DB8-458A-4FB0-945B-9010A7B1D164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D05B144-6633-4FE1-8801-02EE7A981B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="2220" windowWidth="21180" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
+    <workbookView xWindow="8985" yWindow="1575" windowWidth="21180" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>day</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/contains-duplicate-ii/submissions/1089436185/</t>
+  </si>
+  <si>
+    <t>Count Complete Tree Nodes</t>
   </si>
 </sst>
 </file>
@@ -763,7 +766,7 @@
   <dimension ref="A2:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,6 +2121,12 @@
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2175,9 +2184,10 @@
     <hyperlink ref="B52" r:id="rId31" display="https://leetcode.com/problems/reverse-linked-list/" xr:uid="{64BAC716-BDC1-4071-B01E-7D14E2F1B268}"/>
     <hyperlink ref="B53" r:id="rId32" display="https://leetcode.com/problems/contains-duplicate/" xr:uid="{D0DA0E09-DFDD-4ED0-B693-CE37AFAB4DD7}"/>
     <hyperlink ref="B54" r:id="rId33" display="https://leetcode.com/problems/contains-duplicate-ii/" xr:uid="{19925A9D-0321-4E3A-998D-58DC83F31963}"/>
+    <hyperlink ref="B55" r:id="rId34" display="https://leetcode.com/problems/count-complete-tree-nodes/" xr:uid="{8C0EDE32-7283-442E-B70B-2F12EFA46E05}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId34"/>
+  <pageSetup orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
 
@@ -2225,7 +2235,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.80392156862745101</v>
+        <v>0.78846153846153844</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>

</xml_diff>

<commit_message>
building a simple obj
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D05B144-6633-4FE1-8801-02EE7A981B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29696E1A-AB85-4F1E-B26B-36F71E7CBCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8985" yWindow="1575" windowWidth="21180" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
+    <workbookView xWindow="1275" yWindow="1020" windowWidth="21180" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>day</t>
   </si>
@@ -382,6 +382,12 @@
   </si>
   <si>
     <t>Count Complete Tree Nodes</t>
+  </si>
+  <si>
+    <t>Implement Stack using Queues</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-stack-using-queues/submissions/1090591964/</t>
   </si>
 </sst>
 </file>
@@ -765,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECC8050-3973-4D61-AD7A-348E46DD3771}">
   <dimension ref="A2:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,6 +2138,18 @@
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="I56" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2185,9 +2203,10 @@
     <hyperlink ref="B53" r:id="rId32" display="https://leetcode.com/problems/contains-duplicate/" xr:uid="{D0DA0E09-DFDD-4ED0-B693-CE37AFAB4DD7}"/>
     <hyperlink ref="B54" r:id="rId33" display="https://leetcode.com/problems/contains-duplicate-ii/" xr:uid="{19925A9D-0321-4E3A-998D-58DC83F31963}"/>
     <hyperlink ref="B55" r:id="rId34" display="https://leetcode.com/problems/count-complete-tree-nodes/" xr:uid="{8C0EDE32-7283-442E-B70B-2F12EFA46E05}"/>
+    <hyperlink ref="B56" r:id="rId35" display="https://leetcode.com/problems/implement-stack-using-queues/" xr:uid="{4D882F15-A42E-4A41-84DF-B7AF5BB3A9F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId35"/>
+  <pageSetup orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
 
@@ -2235,11 +2254,11 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.78846153846153844</v>
+        <v>0.79245283018867929</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>
-        <v>1.5853658536585367</v>
+        <v>1.5714285714285714</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(List!E3:E500)/COUNT(List!E3:E500)</f>

</xml_diff>

<commit_message>
tree never used to it
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29696E1A-AB85-4F1E-B26B-36F71E7CBCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248B18A6-4739-4698-B07C-A8A874CF789D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="1020" windowWidth="21180" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>day</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/implement-stack-using-queues/submissions/1090591964/</t>
+  </si>
+  <si>
+    <t>Invert Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -772,7 +775,7 @@
   <dimension ref="A2:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2155,6 +2158,12 @@
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2204,9 +2213,10 @@
     <hyperlink ref="B54" r:id="rId33" display="https://leetcode.com/problems/contains-duplicate-ii/" xr:uid="{19925A9D-0321-4E3A-998D-58DC83F31963}"/>
     <hyperlink ref="B55" r:id="rId34" display="https://leetcode.com/problems/count-complete-tree-nodes/" xr:uid="{8C0EDE32-7283-442E-B70B-2F12EFA46E05}"/>
     <hyperlink ref="B56" r:id="rId35" display="https://leetcode.com/problems/implement-stack-using-queues/" xr:uid="{4D882F15-A42E-4A41-84DF-B7AF5BB3A9F2}"/>
+    <hyperlink ref="B57" r:id="rId36" display="https://leetcode.com/problems/invert-binary-tree/" xr:uid="{76CBC250-AA98-4584-A372-942F619A46ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
 
@@ -2254,7 +2264,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.79245283018867929</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>

</xml_diff>

<commit_message>
recursion approach was fantastic!
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB4B2A2-9072-4E8C-9D7B-C4FADD8353B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF802C0-A7FA-4ABE-914A-B7DE038F804D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>day</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/summary-ranges/submissions/1092074327/</t>
+  </si>
+  <si>
+    <t>Power of Two</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/power-of-two/submissions/1093210199/</t>
   </si>
 </sst>
 </file>
@@ -778,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECC8050-3973-4D61-AD7A-348E46DD3771}">
-  <dimension ref="A2:J59"/>
+  <dimension ref="A2:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,6 +2198,108 @@
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="I59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2233,9 +2341,10 @@
     <hyperlink ref="B56" r:id="rId35" display="https://leetcode.com/problems/implement-stack-using-queues/" xr:uid="{4D882F15-A42E-4A41-84DF-B7AF5BB3A9F2}"/>
     <hyperlink ref="B57" r:id="rId36" display="https://leetcode.com/problems/invert-binary-tree/" xr:uid="{76CBC250-AA98-4584-A372-942F619A46ED}"/>
     <hyperlink ref="B58" r:id="rId37" display="https://leetcode.com/problems/summary-ranges/" xr:uid="{7E475741-16D3-4F0C-A35E-4A720D7A6C91}"/>
+    <hyperlink ref="B59" r:id="rId38" display="https://leetcode.com/problems/power-of-two/" xr:uid="{95B3BD69-45E8-4868-999A-E94BA0458ACF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId38"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
 
@@ -2243,8 +2352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474C32BF-24AC-4A70-BA6A-73A9C2809AF6}">
   <dimension ref="A2:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2283,11 +2392,11 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.78181818181818186</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>
-        <v>1.5813953488372092</v>
+        <v>1.5681818181818181</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(List!E3:E500)/COUNT(List!E3:E500)</f>

</xml_diff>

<commit_message>
recursion and binary tree practice required
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC4A470-113B-4DAB-A047-CF5FAC97AFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457EC2C7-9A78-4B9D-AD4F-5AC27167B55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="645" yWindow="675" windowWidth="25815" windowHeight="13845" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t>day</t>
   </si>
@@ -421,6 +421,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/valid-anagram/submissions/1095286693/</t>
+  </si>
+  <si>
+    <t>Binary Tree Paths</t>
   </si>
 </sst>
 </file>
@@ -804,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECC8050-3973-4D61-AD7A-348E46DD3771}">
   <dimension ref="A2:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,6 +2287,12 @@
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2399,9 +2408,10 @@
     <hyperlink ref="B60" r:id="rId39" display="https://leetcode.com/problems/implement-queue-using-stacks/" xr:uid="{4F04CE6B-4190-4D2B-A755-267C5B90163C}"/>
     <hyperlink ref="B61" r:id="rId40" display="https://leetcode.com/problems/palindrome-linked-list/" xr:uid="{BC7D1DD3-25C9-4DF3-88E3-565F52A2CC99}"/>
     <hyperlink ref="B62" r:id="rId41" display="https://leetcode.com/problems/valid-anagram/" xr:uid="{A8962A75-067B-445A-89B6-53480A991FB9}"/>
+    <hyperlink ref="B63" r:id="rId42" display="https://leetcode.com/problems/binary-tree-paths/" xr:uid="{206B0DF0-9222-45C4-B0DC-B529A6702C0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId42"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
 
@@ -2449,7 +2459,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.81355932203389836</v>
+        <v>0.8</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>

</xml_diff>

<commit_message>
two pointers, in-place algo
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD21508-EB5B-46A3-AA40-4641E5F79448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEE9D76-C82D-4951-B743-518F2EC22F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t>day</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/first-bad-version/submissions/1098993829/</t>
+  </si>
+  <si>
+    <t>Move Zeroes</t>
   </si>
 </sst>
 </file>
@@ -829,7 +832,7 @@
   <dimension ref="A2:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2381,6 +2384,12 @@
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -2476,9 +2485,10 @@
     <hyperlink ref="B65" r:id="rId44" display="https://leetcode.com/problems/ugly-number/" xr:uid="{612DEA76-71A9-4BA2-A041-CD635A545A7D}"/>
     <hyperlink ref="B66" r:id="rId45" display="https://leetcode.com/problems/missing-number/" xr:uid="{32150D65-6943-4D95-9C35-4CF854A953AE}"/>
     <hyperlink ref="B67" r:id="rId46" display="https://leetcode.com/problems/first-bad-version/" xr:uid="{E295D543-822D-43B6-894E-C3DAC2F0B6CD}"/>
+    <hyperlink ref="B68" r:id="rId47" display="https://leetcode.com/problems/move-zeroes/" xr:uid="{3ECE3C48-C3DD-4B86-8A0B-FDAB03EA1CD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId47"/>
+  <pageSetup orientation="portrait" r:id="rId48"/>
 </worksheet>
 </file>
 
@@ -2526,7 +2536,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.796875</v>
+        <v>0.7846153846153846</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>

</xml_diff>

<commit_message>
math is faster than numpy
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4244743-2EBA-4BCC-8E47-029AA1462879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C0ECF2-8CA5-4C0C-9F94-BF990E71D75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="660" windowWidth="25815" windowHeight="13350" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
   <si>
     <t>day</t>
   </si>
@@ -478,6 +478,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/counting-bits/submissions/1103572384/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/power-of-four/submissions/1104502549/</t>
+  </si>
+  <si>
+    <t>Power of Four</t>
   </si>
 </sst>
 </file>
@@ -861,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECC8050-3973-4D61-AD7A-348E46DD3771}">
   <dimension ref="A2:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="I84" sqref="I84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2510,6 +2516,18 @@
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="I74" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -2581,9 +2599,10 @@
     <hyperlink ref="B71" r:id="rId50" display="https://leetcode.com/problems/range-sum-query-immutable/" xr:uid="{9E26BA42-0548-47F7-959E-483987C5A78C}"/>
     <hyperlink ref="B72" r:id="rId51" display="https://leetcode.com/problems/power-of-three/" xr:uid="{69B30FDE-388F-4D7A-BB38-C07F96CD7D4A}"/>
     <hyperlink ref="B73" r:id="rId52" display="https://leetcode.com/problems/counting-bits/" xr:uid="{7D3CDC68-E08C-41C4-A5B5-9E977ED87388}"/>
+    <hyperlink ref="B74" r:id="rId53" display="https://leetcode.com/problems/power-of-four/" xr:uid="{FE36CD04-D5AD-4BCB-96D9-8C4A14874EDA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId53"/>
+  <pageSetup orientation="portrait" r:id="rId54"/>
 </worksheet>
 </file>
 
@@ -2631,11 +2650,11 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.7857142857142857</v>
+        <v>0.78873239436619713</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>
-        <v>1.5272727272727273</v>
+        <v>1.5178571428571428</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(List!E3:E500)/COUNT(List!E3:E500)</f>

</xml_diff>

<commit_message>
focused on quick completion, poor answer
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D9B73F-6AF0-490B-A7B9-74B4905214F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79017ABB-B845-429E-A161-AE24EB11D99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="660" windowWidth="25815" windowHeight="13350" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
   <si>
     <t>day</t>
   </si>
@@ -490,6 +490,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/reverse-string/submissions/1104962422/</t>
+  </si>
+  <si>
+    <t>Reverse Vowels of a String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-vowels-of-a-string/submissions/1105788750/</t>
   </si>
 </sst>
 </file>
@@ -874,7 +880,7 @@
   <dimension ref="A2:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+      <selection activeCell="J76" sqref="J76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2556,6 +2562,18 @@
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="I76" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -2619,9 +2637,10 @@
     <hyperlink ref="B73" r:id="rId52" display="https://leetcode.com/problems/counting-bits/" xr:uid="{7D3CDC68-E08C-41C4-A5B5-9E977ED87388}"/>
     <hyperlink ref="B74" r:id="rId53" display="https://leetcode.com/problems/power-of-four/" xr:uid="{FE36CD04-D5AD-4BCB-96D9-8C4A14874EDA}"/>
     <hyperlink ref="B75" r:id="rId54" display="https://leetcode.com/problems/reverse-string/" xr:uid="{1EAF4BE5-B1CF-429F-ADE1-96BAA47BAD85}"/>
+    <hyperlink ref="B76" r:id="rId55" display="https://leetcode.com/problems/reverse-vowels-of-a-string/" xr:uid="{A544B11B-B818-49D5-AA8F-AA06941CFCB8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId55"/>
+  <pageSetup orientation="portrait" r:id="rId56"/>
 </worksheet>
 </file>
 
@@ -2669,11 +2688,11 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.79166666666666663</v>
+        <v>0.79452054794520544</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>
-        <v>1.5087719298245614</v>
+        <v>1.5172413793103448</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(List!E3:E500)/COUNT(List!E3:E500)</f>

</xml_diff>

<commit_message>
work resumed - back from vacation
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79017ABB-B845-429E-A161-AE24EB11D99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E51DCA5-4FB1-4611-BDF5-2234C0819DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="660" windowWidth="25815" windowHeight="13350" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
+    <workbookView xWindow="1725" yWindow="810" windowWidth="25815" windowHeight="13350" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
   <si>
     <t>day</t>
   </si>
@@ -496,6 +496,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/reverse-vowels-of-a-string/submissions/1105788750/</t>
+  </si>
+  <si>
+    <t>Ransom Note</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/ransom-note/submissions/1119784137/</t>
   </si>
 </sst>
 </file>
@@ -880,7 +886,7 @@
   <dimension ref="A2:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J76" sqref="J76"/>
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2579,6 +2585,18 @@
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="I77" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2638,9 +2656,10 @@
     <hyperlink ref="B74" r:id="rId53" display="https://leetcode.com/problems/power-of-four/" xr:uid="{FE36CD04-D5AD-4BCB-96D9-8C4A14874EDA}"/>
     <hyperlink ref="B75" r:id="rId54" display="https://leetcode.com/problems/reverse-string/" xr:uid="{1EAF4BE5-B1CF-429F-ADE1-96BAA47BAD85}"/>
     <hyperlink ref="B76" r:id="rId55" display="https://leetcode.com/problems/reverse-vowels-of-a-string/" xr:uid="{A544B11B-B818-49D5-AA8F-AA06941CFCB8}"/>
+    <hyperlink ref="B77" r:id="rId56" display="https://leetcode.com/problems/ransom-note/" xr:uid="{FAB5A3E7-D1A5-49FD-9B45-856066ECE103}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId56"/>
+  <pageSetup orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
 
@@ -2688,11 +2707,11 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.79452054794520544</v>
+        <v>0.79729729729729726</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>
-        <v>1.5172413793103448</v>
+        <v>1.5254237288135593</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(List!E3:E500)/COUNT(List!E3:E500)</f>

</xml_diff>

<commit_message>
need more hard coding skills
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13A1B49-8EB3-4D1A-ACE5-C79EE022F63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA0A9D0-8EBA-4B4F-B7A9-0B0F0E980217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1725" yWindow="810" windowWidth="25815" windowHeight="13350" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
   <si>
     <t>day</t>
   </si>
@@ -547,6 +547,9 @@
   </si>
   <si>
     <t>Sum of Left Leaves</t>
+  </si>
+  <si>
+    <t>Convert a Number to Hexadecimal</t>
   </si>
 </sst>
 </file>
@@ -931,7 +934,7 @@
   <dimension ref="A2:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2777,6 +2780,12 @@
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -2870,9 +2879,10 @@
     <hyperlink ref="B83" r:id="rId62" display="https://leetcode.com/problems/is-subsequence/" xr:uid="{A3CA29CB-659B-44EF-A562-09D4950B36A2}"/>
     <hyperlink ref="B84" r:id="rId63" display="https://leetcode.com/problems/binary-watch/" xr:uid="{DE864E7C-D7D7-4F20-AF57-126C514A50F2}"/>
     <hyperlink ref="B85" r:id="rId64" display="https://leetcode.com/problems/sum-of-left-leaves/" xr:uid="{5CFAA41B-1494-485F-8E55-AC2C68CE485E}"/>
+    <hyperlink ref="B86" r:id="rId65" display="https://leetcode.com/problems/convert-a-number-to-hexadecimal/" xr:uid="{FECD9F98-159D-4E15-8BFF-288282FFE188}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId65"/>
+  <pageSetup orientation="portrait" r:id="rId66"/>
 </worksheet>
 </file>
 
@@ -2920,7 +2930,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.80487804878048785</v>
+        <v>0.79518072289156627</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>

</xml_diff>

<commit_message>
Counter and sorted with switch
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA0A9D0-8EBA-4B4F-B7A9-0B0F0E980217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B933D519-617B-461E-94F4-11503570EE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1725" yWindow="810" windowWidth="25815" windowHeight="13350" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
   <si>
     <t>day</t>
   </si>
@@ -550,6 +550,12 @@
   </si>
   <si>
     <t>Convert a Number to Hexadecimal</t>
+  </si>
+  <si>
+    <t>Longest Palindrome</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-palindrome/submissions/1125227371/</t>
   </si>
 </sst>
 </file>
@@ -934,7 +940,7 @@
   <dimension ref="A2:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2791,6 +2797,18 @@
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>3</v>
+      </c>
+      <c r="I87" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -2880,9 +2898,10 @@
     <hyperlink ref="B84" r:id="rId63" display="https://leetcode.com/problems/binary-watch/" xr:uid="{DE864E7C-D7D7-4F20-AF57-126C514A50F2}"/>
     <hyperlink ref="B85" r:id="rId64" display="https://leetcode.com/problems/sum-of-left-leaves/" xr:uid="{5CFAA41B-1494-485F-8E55-AC2C68CE485E}"/>
     <hyperlink ref="B86" r:id="rId65" display="https://leetcode.com/problems/convert-a-number-to-hexadecimal/" xr:uid="{FECD9F98-159D-4E15-8BFF-288282FFE188}"/>
+    <hyperlink ref="B87" r:id="rId66" display="https://leetcode.com/problems/longest-palindrome/" xr:uid="{3EF32C8C-C3A8-4CB3-B58E-5188ECBB7815}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId66"/>
+  <pageSetup orientation="portrait" r:id="rId67"/>
 </worksheet>
 </file>
 
@@ -2930,11 +2949,11 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.79518072289156627</v>
+        <v>0.79761904761904767</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>
-        <v>1.606060606060606</v>
+        <v>1.6268656716417911</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(List!E3:E500)/COUNT(List!E3:E500)</f>

</xml_diff>

<commit_message>
pattern by *2 and strip side
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D652AF13-E667-483A-8E54-C6C42E168D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F50FDB9-865E-4101-BE87-878D3EA13783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29970" yWindow="1155" windowWidth="21600" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
   <si>
     <t>day</t>
   </si>
@@ -595,6 +595,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/assign-cookies/submissions/1131802204/</t>
+  </si>
+  <si>
+    <t>Repeated Substring Pattern</t>
   </si>
 </sst>
 </file>
@@ -979,7 +982,7 @@
   <dimension ref="A2:J110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2966,6 +2969,12 @@
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -3118,9 +3127,10 @@
     <hyperlink ref="B92" r:id="rId71" display="https://leetcode.com/problems/arranging-coins" xr:uid="{EA4D99AD-4C43-4EA6-A39F-55272757B88B}"/>
     <hyperlink ref="B93" r:id="rId72" display="https://leetcode.com/problems/find-all-numbers-disappeared-in-an-array/" xr:uid="{A3F26AF2-B321-4B61-8202-D77B85480E51}"/>
     <hyperlink ref="B94" r:id="rId73" display="https://leetcode.com/problems/assign-cookies/" xr:uid="{31D49D3A-2247-4BCE-9F37-899210C1E9F3}"/>
+    <hyperlink ref="B95" r:id="rId74" display="https://leetcode.com/problems/repeated-substring-pattern/" xr:uid="{6E6C5A47-8F7F-441D-893D-CBEEB4410F61}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId74"/>
+  <pageSetup orientation="portrait" r:id="rId75"/>
 </worksheet>
 </file>
 
@@ -3168,7 +3178,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.80219780219780223</v>
+        <v>0.79347826086956519</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>

</xml_diff>

<commit_message>
bits and pieces comparison
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F50FDB9-865E-4101-BE87-878D3EA13783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6B7011-61E7-4BC3-8DDA-D870060A8844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29970" yWindow="1155" windowWidth="21600" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
   <si>
     <t>day</t>
   </si>
@@ -598,6 +598,12 @@
   </si>
   <si>
     <t>Repeated Substring Pattern</t>
+  </si>
+  <si>
+    <t>Hamming Distance</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/hamming-distance/submissions/1133279332/</t>
   </si>
 </sst>
 </file>
@@ -982,7 +988,7 @@
   <dimension ref="A2:J110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="F95" sqref="F95"/>
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2980,6 +2986,18 @@
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="I96" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
@@ -3128,9 +3146,10 @@
     <hyperlink ref="B93" r:id="rId72" display="https://leetcode.com/problems/find-all-numbers-disappeared-in-an-array/" xr:uid="{A3F26AF2-B321-4B61-8202-D77B85480E51}"/>
     <hyperlink ref="B94" r:id="rId73" display="https://leetcode.com/problems/assign-cookies/" xr:uid="{31D49D3A-2247-4BCE-9F37-899210C1E9F3}"/>
     <hyperlink ref="B95" r:id="rId74" display="https://leetcode.com/problems/repeated-substring-pattern/" xr:uid="{6E6C5A47-8F7F-441D-893D-CBEEB4410F61}"/>
+    <hyperlink ref="B96" r:id="rId75" display="https://leetcode.com/problems/hamming-distance/" xr:uid="{A26CAB14-F45C-4CFA-90AB-19E4070B9837}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId75"/>
+  <pageSetup orientation="portrait" r:id="rId76"/>
 </worksheet>
 </file>
 
@@ -3178,11 +3197,11 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.79347826086956519</v>
+        <v>0.79569892473118276</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>
-        <v>1.6027397260273972</v>
+        <v>1.5945945945945945</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(List!E3:E500)/COUNT(List!E3:E500)</f>

</xml_diff>

<commit_message>
bin and int binary
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3500BDF7-F913-426D-B0AA-2172BD521621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F210D93F-DF60-43E3-83D6-76052DD48904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29970" yWindow="1155" windowWidth="21600" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
   <si>
     <t>day</t>
   </si>
@@ -607,6 +607,12 @@
   </si>
   <si>
     <t>Island Perimeter</t>
+  </si>
+  <si>
+    <t>Number Complement</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-complement/submissions/1140051188/</t>
   </si>
 </sst>
 </file>
@@ -990,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECC8050-3973-4D61-AD7A-348E46DD3771}">
   <dimension ref="A2:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E96" sqref="E96"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3003,7 +3009,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -3014,67 +3020,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B98" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="I98" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>108</v>
       </c>
@@ -3157,9 +3175,10 @@
     <hyperlink ref="B95" r:id="rId74" display="https://leetcode.com/problems/repeated-substring-pattern/" xr:uid="{6E6C5A47-8F7F-441D-893D-CBEEB4410F61}"/>
     <hyperlink ref="B96" r:id="rId75" display="https://leetcode.com/problems/hamming-distance/" xr:uid="{A26CAB14-F45C-4CFA-90AB-19E4070B9837}"/>
     <hyperlink ref="B97" r:id="rId76" display="https://leetcode.com/problems/island-perimeter/" xr:uid="{AC248191-C91D-4EB1-8DCE-0FD2EF83FE99}"/>
+    <hyperlink ref="B98" r:id="rId77" display="https://leetcode.com/problems/number-complement/" xr:uid="{67355069-170D-4EC4-AE5E-4E1093D068AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId77"/>
+  <pageSetup orientation="portrait" r:id="rId78"/>
 </worksheet>
 </file>
 
@@ -3207,11 +3226,11 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.78723404255319152</v>
+        <v>0.78947368421052633</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>
-        <v>1.5945945945945945</v>
+        <v>1.5866666666666667</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(List!E3:E500)/COUNT(List!E3:E500)</f>

</xml_diff>

<commit_message>
replace, upper, and join
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F210D93F-DF60-43E3-83D6-76052DD48904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D399F5-9285-443C-AE25-7492C742E1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29970" yWindow="1155" windowWidth="21600" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
   <si>
     <t>day</t>
   </si>
@@ -613,6 +613,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/number-complement/submissions/1140051188/</t>
+  </si>
+  <si>
+    <t>License Key Formatting</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/license-key-formatting/submissions/1140947621/</t>
   </si>
 </sst>
 </file>
@@ -997,7 +1003,7 @@
   <dimension ref="A2:J110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F101" sqref="F101"/>
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3040,6 +3046,18 @@
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
+      <c r="I99" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -3176,9 +3194,10 @@
     <hyperlink ref="B96" r:id="rId75" display="https://leetcode.com/problems/hamming-distance/" xr:uid="{A26CAB14-F45C-4CFA-90AB-19E4070B9837}"/>
     <hyperlink ref="B97" r:id="rId76" display="https://leetcode.com/problems/island-perimeter/" xr:uid="{AC248191-C91D-4EB1-8DCE-0FD2EF83FE99}"/>
     <hyperlink ref="B98" r:id="rId77" display="https://leetcode.com/problems/number-complement/" xr:uid="{67355069-170D-4EC4-AE5E-4E1093D068AC}"/>
+    <hyperlink ref="B99" r:id="rId78" display="https://leetcode.com/problems/license-key-formatting/" xr:uid="{FB5D85AB-A0BE-4C77-AF8C-6984D3FAAE46}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId78"/>
+  <pageSetup orientation="portrait" r:id="rId79"/>
 </worksheet>
 </file>
 
@@ -3226,11 +3245,11 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.78947368421052633</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>
-        <v>1.5866666666666667</v>
+        <v>1.5921052631578947</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(List!E3:E500)/COUNT(List!E3:E500)</f>

</xml_diff>

<commit_message>
O(n) and simple comparison
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D399F5-9285-443C-AE25-7492C742E1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B886C0A-BC47-4A0D-AB5B-02DC772567CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29970" yWindow="1155" windowWidth="21600" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t>day</t>
   </si>
@@ -619,6 +619,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/license-key-formatting/submissions/1140947621/</t>
+  </si>
+  <si>
+    <t>Max Consecutive Ones</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/max-consecutive-ones/submissions/1141416344/</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1009,7 @@
   <dimension ref="A2:J110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3063,6 +3069,18 @@
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>2</v>
+      </c>
+      <c r="I100" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -3195,9 +3213,10 @@
     <hyperlink ref="B97" r:id="rId76" display="https://leetcode.com/problems/island-perimeter/" xr:uid="{AC248191-C91D-4EB1-8DCE-0FD2EF83FE99}"/>
     <hyperlink ref="B98" r:id="rId77" display="https://leetcode.com/problems/number-complement/" xr:uid="{67355069-170D-4EC4-AE5E-4E1093D068AC}"/>
     <hyperlink ref="B99" r:id="rId78" display="https://leetcode.com/problems/license-key-formatting/" xr:uid="{FB5D85AB-A0BE-4C77-AF8C-6984D3FAAE46}"/>
+    <hyperlink ref="B100" r:id="rId79" display="https://leetcode.com/problems/max-consecutive-ones/" xr:uid="{973831A7-A160-4232-BBB9-ED3207AE5874}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId79"/>
+  <pageSetup orientation="portrait" r:id="rId80"/>
 </worksheet>
 </file>
 
@@ -3245,11 +3264,11 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.79166666666666663</v>
+        <v>0.79381443298969068</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>
-        <v>1.5921052631578947</v>
+        <v>1.5974025974025974</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(List!E3:E500)/COUNT(List!E3:E500)</f>

</xml_diff>

<commit_message>
square and O(n) iteration
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B886C0A-BC47-4A0D-AB5B-02DC772567CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31ECEB3-BE0D-4516-97F6-87279439E1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29970" yWindow="1155" windowWidth="21600" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="198">
   <si>
     <t>day</t>
   </si>
@@ -625,6 +625,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/max-consecutive-ones/submissions/1141416344/</t>
+  </si>
+  <si>
+    <t>Construct the Rectangle</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/construct-the-rectangle/submissions/1142907874/</t>
   </si>
 </sst>
 </file>
@@ -710,9 +716,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -750,7 +756,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -856,7 +862,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -998,7 +1004,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1009,7 +1015,7 @@
   <dimension ref="A2:J110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+      <selection activeCell="G105" sqref="G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3086,6 +3092,18 @@
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="I101" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -3214,9 +3232,10 @@
     <hyperlink ref="B98" r:id="rId77" display="https://leetcode.com/problems/number-complement/" xr:uid="{67355069-170D-4EC4-AE5E-4E1093D068AC}"/>
     <hyperlink ref="B99" r:id="rId78" display="https://leetcode.com/problems/license-key-formatting/" xr:uid="{FB5D85AB-A0BE-4C77-AF8C-6984D3FAAE46}"/>
     <hyperlink ref="B100" r:id="rId79" display="https://leetcode.com/problems/max-consecutive-ones/" xr:uid="{973831A7-A160-4232-BBB9-ED3207AE5874}"/>
+    <hyperlink ref="B101" r:id="rId80" display="https://leetcode.com/problems/construct-the-rectangle/" xr:uid="{F6BCAB0F-0842-4A36-8BA4-AF7A4ED9BAA4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId80"/>
+  <pageSetup orientation="portrait" r:id="rId81"/>
 </worksheet>
 </file>
 
@@ -3264,11 +3283,11 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.79381443298969068</v>
+        <v>0.79591836734693877</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>
-        <v>1.5974025974025974</v>
+        <v>1.5897435897435896</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(List!E3:E500)/COUNT(List!E3:E500)</f>

</xml_diff>

<commit_message>
logic was right, weren't able to code to work
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4162555C-7B08-4EA6-81DF-DD9FA8534153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B6FCA5-6E98-49BF-AAE8-364835C3C73D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
   <si>
     <t>day</t>
   </si>
@@ -649,6 +649,9 @@
   </si>
   <si>
     <t>Longest Palindromic Substring</t>
+  </si>
+  <si>
+    <t>Zigzag Conversion</t>
   </si>
 </sst>
 </file>
@@ -3181,6 +3184,12 @@
       <c r="A106">
         <v>104</v>
       </c>
+      <c r="B106" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107">
@@ -3288,9 +3297,10 @@
     <hyperlink ref="B103" r:id="rId82" display="https://leetcode.com/problems/add-two-numbers/" xr:uid="{EE0C5171-8AAD-465C-BCED-2646A859BCBF}"/>
     <hyperlink ref="B104" r:id="rId83" display="https://leetcode.com/problems/longest-substring-without-repeating-characters/" xr:uid="{6AFB477D-815D-418E-8877-EC0C7119EFF7}"/>
     <hyperlink ref="B105" r:id="rId84" display="https://leetcode.com/problems/longest-palindromic-substring/" xr:uid="{D6B17B77-0330-4EA1-98D9-4792AD957D36}"/>
+    <hyperlink ref="B106" r:id="rId85" display="https://leetcode.com/problems/zigzag-conversion/" xr:uid="{75FD37B5-BD0C-4BBD-B9DE-810195B76E84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId85"/>
+  <pageSetup orientation="portrait" r:id="rId86"/>
 </worksheet>
 </file>
 
@@ -3338,7 +3348,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.77450980392156865</v>
+        <v>0.76699029126213591</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>

</xml_diff>

<commit_message>
need review for mid level questions
</commit_message>
<xml_diff>
--- a/LeetCodeStats.xlsx
+++ b/LeetCodeStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongwoo Daniel Kang\Desktop\D\CodingPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A7B46C-92C1-4B8D-A53F-1C1833F13369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFD5CA8-1551-433D-AC3F-C67181D97286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2E8680C6-7AA1-4EFA-B278-DAF62749C3B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="208">
   <si>
     <t>day</t>
   </si>
@@ -658,6 +658,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/reverse-integer/submissions/1154054610/</t>
+  </si>
+  <si>
+    <t>String to Integer (atoi)</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1045,7 @@
   <dimension ref="A2:J110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F113" sqref="F113"/>
+      <selection activeCell="F114" sqref="F114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3217,6 +3220,12 @@
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -3317,9 +3326,10 @@
     <hyperlink ref="B105" r:id="rId84" display="https://leetcode.com/problems/longest-palindromic-substring/" xr:uid="{D6B17B77-0330-4EA1-98D9-4792AD957D36}"/>
     <hyperlink ref="B106" r:id="rId85" display="https://leetcode.com/problems/zigzag-conversion/" xr:uid="{75FD37B5-BD0C-4BBD-B9DE-810195B76E84}"/>
     <hyperlink ref="B107" r:id="rId86" display="https://leetcode.com/problems/reverse-integer/" xr:uid="{476F2089-E47E-4786-845D-5D16DCADC0B6}"/>
+    <hyperlink ref="B108" r:id="rId87" display="https://leetcode.com/problems/string-to-integer-atoi/" xr:uid="{785D1968-4290-49E7-84F3-A9F098E73BFC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId87"/>
+  <pageSetup orientation="portrait" r:id="rId88"/>
 </worksheet>
 </file>
 
@@ -3367,7 +3377,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <f>SUM(List!C3:C500)/COUNT(List!C3:C500)</f>
-        <v>0.76923076923076927</v>
+        <v>0.76190476190476186</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(List!D3:D500)/COUNT(List!D3:D500)</f>

</xml_diff>